<commit_message>
Fixed keys of array and NULL
</commit_message>
<xml_diff>
--- a/Tasks/Task5/График.xlsx
+++ b/Tasks/Task5/График.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CLionProjects\AlgorithmsPhilush\Tasks\Task5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A132EC28-57BA-4C9B-9F6C-1A9EAB22554E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E30EB6-E2AB-4BA9-BA38-FBF3D1EF093A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33045" yWindow="2445" windowWidth="22200" windowHeight="11835" xr2:uid="{0C689934-A993-4314-8898-DD16A6A48349}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>высота</t>
   </si>
   <si>
-    <t>время поиска 10  элементов</t>
+    <t>array</t>
+  </si>
+  <si>
+    <t>map</t>
   </si>
 </sst>
 </file>
@@ -110,6 +113,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Добавление</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -154,7 +182,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>время поиска 10  элементов</c:v>
+                  <c:v>array</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -253,64 +281,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0002</c:v>
+                  <c:v>12.9999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9984999999999999</c:v>
+                  <c:v>25.9998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9988000000000001</c:v>
+                  <c:v>45.970799999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0001999999999995</c:v>
+                  <c:v>59.000300000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9970999999999997</c:v>
+                  <c:v>72.9983</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.998900000000001</c:v>
+                  <c:v>84.000299999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.999499999999999</c:v>
+                  <c:v>97.000100000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.9984</c:v>
+                  <c:v>110.9689</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.9985</c:v>
+                  <c:v>134.97280000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.998799999999999</c:v>
+                  <c:v>134.97290000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.9861</c:v>
+                  <c:v>151.00020000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.998999999999999</c:v>
+                  <c:v>168.99979999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.999700000000001</c:v>
+                  <c:v>182.98009999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26.9983</c:v>
+                  <c:v>214.99950000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.997800000000002</c:v>
+                  <c:v>224.20840000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.998699999999999</c:v>
+                  <c:v>219.00710000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.998399999999997</c:v>
+                  <c:v>227.9708</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.998100000000001</c:v>
+                  <c:v>241.0051</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>38.9681</c:v>
+                  <c:v>252.7825</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>39.997900000000001</c:v>
+                  <c:v>264.99759999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -318,7 +346,184 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-12CD-40AB-A33D-3A3F5A782686}"/>
+              <c16:uniqueId val="{00000000-5869-4D78-B819-4D55E8CFE1D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>550000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>650000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>850000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$D$2:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.999600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.998600000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.969200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.9997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142.99889999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171.99879999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>203.00110000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>241.99879999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>295.99849999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>328.00060000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>365.00139999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>404.09059999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>425.50650000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>457.00220000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>487.03809999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>517.99919999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>545.10059999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>584.78219999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>622.99599999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5869-4D78-B819-4D55E8CFE1D2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -330,11 +535,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1588114911"/>
-        <c:axId val="1588113247"/>
+        <c:axId val="13531296"/>
+        <c:axId val="13538368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1588114911"/>
+        <c:axId val="13531296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,12 +596,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588113247"/>
+        <c:crossAx val="13538368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1588113247"/>
+        <c:axId val="13538368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,7 +658,478 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588114911"/>
+        <c:crossAx val="13531296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>поиск</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>550000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>650000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>850000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$E$2:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0023999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.998900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0002000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9984999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.000699999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.0002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.000799999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.000599999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.024299999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.999099999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68.006799999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74.998400000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87.000299999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.003900000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>94.997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99.967200000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>103.99760000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>111.99890000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>118.9987</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>153.0333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DB3-4F2E-A404-BE7574E82917}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="180843616"/>
+        <c:axId val="180849024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="180843616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180849024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="180849024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180843616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -549,6 +1225,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1065,27 +1781,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1">
+        <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E87EDE-2686-4467-A6A6-73525DDD61A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{026F6B6F-D0CD-4F69-9DA1-8540FA08F8DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1098,6 +2330,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B60E53B9-E88C-4D19-9A57-19403F6AC87B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1403,23 +2671,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1DF7B3-DBCB-4387-A8CF-5164F7CDBAB0}">
-  <dimension ref="B1:C22"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <f>(ROW() - 2) * 50000</f>
         <v>0</v>
@@ -1427,185 +2709,374 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>(ROW() - 2) * 50000</f>
         <v>50000</v>
       </c>
       <c r="C3">
-        <v>2.0002</v>
+        <v>12.9999</v>
+      </c>
+      <c r="D3">
+        <v>25.999600000000001</v>
+      </c>
+      <c r="E3">
+        <v>5.0023999999999997</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <f t="shared" ref="B4:B22" si="0">(ROW() - 2) * 50000</f>
         <v>100000</v>
       </c>
       <c r="C4">
-        <v>4.9984999999999999</v>
+        <v>25.9998</v>
+      </c>
+      <c r="D4">
+        <v>53.998600000000003</v>
+      </c>
+      <c r="E4">
+        <v>11.998900000000001</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
       <c r="C5">
-        <v>5.9988000000000001</v>
+        <v>45.970799999999997</v>
+      </c>
+      <c r="D5">
+        <v>82.969200000000001</v>
+      </c>
+      <c r="E5">
+        <v>4.0002000000000004</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
       <c r="C6">
-        <v>8.0001999999999995</v>
+        <v>59.000300000000003</v>
+      </c>
+      <c r="D6">
+        <v>112.9997</v>
+      </c>
+      <c r="E6">
+        <v>9.9984999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
       <c r="C7">
-        <v>9.9970999999999997</v>
+        <v>72.9983</v>
+      </c>
+      <c r="D7">
+        <v>142.99889999999999</v>
+      </c>
+      <c r="E7">
+        <v>18.000699999999998</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="C8">
-        <v>11.998900000000001</v>
+        <v>84.000299999999996</v>
+      </c>
+      <c r="D8">
+        <v>171.99879999999999</v>
+      </c>
+      <c r="E8">
+        <v>24.0002</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>350000</v>
       </c>
       <c r="C9">
-        <v>13.999499999999999</v>
+        <v>97.000100000000003</v>
+      </c>
+      <c r="D9">
+        <v>203.00110000000001</v>
+      </c>
+      <c r="E9">
+        <v>33.000799999999998</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
       <c r="C10">
-        <v>15.9984</v>
+        <v>110.9689</v>
+      </c>
+      <c r="D10">
+        <v>241.99879999999999</v>
+      </c>
+      <c r="E10">
+        <v>38.000599999999999</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>450000</v>
       </c>
       <c r="C11">
-        <v>17.9985</v>
+        <v>134.97280000000001</v>
+      </c>
+      <c r="D11">
+        <v>278</v>
+      </c>
+      <c r="E11">
+        <v>44.024299999999997</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
       <c r="C12">
-        <v>19.998799999999999</v>
+        <v>134.97290000000001</v>
+      </c>
+      <c r="D12">
+        <v>295.99849999999998</v>
+      </c>
+      <c r="E12">
+        <v>60.999099999999999</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>550000</v>
       </c>
       <c r="C13">
-        <v>21.9861</v>
+        <v>151.00020000000001</v>
+      </c>
+      <c r="D13">
+        <v>328.00060000000002</v>
+      </c>
+      <c r="E13">
+        <v>68.006799999999998</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
       <c r="C14">
-        <v>23.998999999999999</v>
+        <v>168.99979999999999</v>
+      </c>
+      <c r="D14">
+        <v>365.00139999999999</v>
+      </c>
+      <c r="E14">
+        <v>74.998400000000004</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>650000</v>
       </c>
       <c r="C15">
-        <v>25.999700000000001</v>
+        <v>182.98009999999999</v>
+      </c>
+      <c r="D15">
+        <v>404.09059999999999</v>
+      </c>
+      <c r="E15">
+        <v>87.000299999999996</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
       <c r="C16">
-        <v>26.9983</v>
+        <v>214.99950000000001</v>
+      </c>
+      <c r="D16">
+        <v>425.50650000000002</v>
+      </c>
+      <c r="E16">
+        <v>88.003900000000002</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>750000</v>
       </c>
       <c r="C17">
-        <v>29.997800000000002</v>
+        <v>224.20840000000001</v>
+      </c>
+      <c r="D17">
+        <v>457.00220000000002</v>
+      </c>
+      <c r="E17">
+        <v>94.997</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>800000</v>
       </c>
       <c r="C18">
-        <v>30.998699999999999</v>
+        <v>219.00710000000001</v>
+      </c>
+      <c r="D18">
+        <v>487.03809999999999</v>
+      </c>
+      <c r="E18">
+        <v>99.967200000000005</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>850000</v>
       </c>
       <c r="C19">
-        <v>32.998399999999997</v>
+        <v>227.9708</v>
+      </c>
+      <c r="D19">
+        <v>517.99919999999997</v>
+      </c>
+      <c r="E19">
+        <v>103.99760000000001</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>900000</v>
       </c>
       <c r="C20">
-        <v>36.998100000000001</v>
+        <v>241.0051</v>
+      </c>
+      <c r="D20">
+        <v>545.10059999999999</v>
+      </c>
+      <c r="E20">
+        <v>111.99890000000001</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>950000</v>
       </c>
       <c r="C21">
-        <v>38.9681</v>
+        <v>252.7825</v>
+      </c>
+      <c r="D21">
+        <v>584.78219999999999</v>
+      </c>
+      <c r="E21">
+        <v>118.9987</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
       <c r="C22">
-        <v>39.997900000000001</v>
+        <v>264.99759999999998</v>
+      </c>
+      <c r="D22">
+        <v>622.99599999999998</v>
+      </c>
+      <c r="E22">
+        <v>153.0333</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed task and Node
</commit_message>
<xml_diff>
--- a/Tasks/Task5/График.xlsx
+++ b/Tasks/Task5/График.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CLionProjects\AlgorithmsPhilush\Tasks\Task5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E30EB6-E2AB-4BA9-BA38-FBF3D1EF093A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050824C6-E8D2-4856-A673-100C199F0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33045" yWindow="2445" windowWidth="22200" windowHeight="11835" xr2:uid="{0C689934-A993-4314-8898-DD16A6A48349}"/>
+    <workbookView xWindow="5145" yWindow="2880" windowWidth="22200" windowHeight="11835" xr2:uid="{0C689934-A993-4314-8898-DD16A6A48349}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -458,64 +458,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.999600000000001</c:v>
+                  <c:v>43.330399999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.998600000000003</c:v>
+                  <c:v>90.049499999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.969200000000001</c:v>
+                  <c:v>136.0608</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>112.9997</c:v>
+                  <c:v>184.1953</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>142.99889999999999</c:v>
+                  <c:v>235.64750000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>171.99879999999999</c:v>
+                  <c:v>285.97190000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>203.00110000000001</c:v>
+                  <c:v>335.30459999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>241.99879999999999</c:v>
+                  <c:v>383.70089999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>278</c:v>
+                  <c:v>438.03129999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>295.99849999999998</c:v>
+                  <c:v>489</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>328.00060000000002</c:v>
+                  <c:v>545.14980000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>365.00139999999999</c:v>
+                  <c:v>591.87840000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>404.09059999999999</c:v>
+                  <c:v>646.94870000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>425.50650000000002</c:v>
+                  <c:v>698.91499999999996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>457.00220000000002</c:v>
+                  <c:v>752.89819999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>487.03809999999999</c:v>
+                  <c:v>804.10159999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>517.99919999999997</c:v>
+                  <c:v>863.16390000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>545.10059999999999</c:v>
+                  <c:v>910.42470000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>584.78219999999999</c:v>
+                  <c:v>966.05039999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>622.99599999999998</c:v>
+                  <c:v>1017.2333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2673,8 +2673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1DF7B3-DBCB-4387-A8CF-5164F7CDBAB0}">
   <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,7 +2728,7 @@
         <v>12.9999</v>
       </c>
       <c r="D3">
-        <v>25.999600000000001</v>
+        <v>43.330399999999997</v>
       </c>
       <c r="E3">
         <v>5.0023999999999997</v>
@@ -2746,7 +2746,7 @@
         <v>25.9998</v>
       </c>
       <c r="D4">
-        <v>53.998600000000003</v>
+        <v>90.049499999999995</v>
       </c>
       <c r="E4">
         <v>11.998900000000001</v>
@@ -2764,7 +2764,7 @@
         <v>45.970799999999997</v>
       </c>
       <c r="D5">
-        <v>82.969200000000001</v>
+        <v>136.0608</v>
       </c>
       <c r="E5">
         <v>4.0002000000000004</v>
@@ -2782,7 +2782,7 @@
         <v>59.000300000000003</v>
       </c>
       <c r="D6">
-        <v>112.9997</v>
+        <v>184.1953</v>
       </c>
       <c r="E6">
         <v>9.9984999999999999</v>
@@ -2800,7 +2800,7 @@
         <v>72.9983</v>
       </c>
       <c r="D7">
-        <v>142.99889999999999</v>
+        <v>235.64750000000001</v>
       </c>
       <c r="E7">
         <v>18.000699999999998</v>
@@ -2818,7 +2818,7 @@
         <v>84.000299999999996</v>
       </c>
       <c r="D8">
-        <v>171.99879999999999</v>
+        <v>285.97190000000001</v>
       </c>
       <c r="E8">
         <v>24.0002</v>
@@ -2836,7 +2836,7 @@
         <v>97.000100000000003</v>
       </c>
       <c r="D9">
-        <v>203.00110000000001</v>
+        <v>335.30459999999999</v>
       </c>
       <c r="E9">
         <v>33.000799999999998</v>
@@ -2854,7 +2854,7 @@
         <v>110.9689</v>
       </c>
       <c r="D10">
-        <v>241.99879999999999</v>
+        <v>383.70089999999999</v>
       </c>
       <c r="E10">
         <v>38.000599999999999</v>
@@ -2872,7 +2872,7 @@
         <v>134.97280000000001</v>
       </c>
       <c r="D11">
-        <v>278</v>
+        <v>438.03129999999999</v>
       </c>
       <c r="E11">
         <v>44.024299999999997</v>
@@ -2890,7 +2890,7 @@
         <v>134.97290000000001</v>
       </c>
       <c r="D12">
-        <v>295.99849999999998</v>
+        <v>489</v>
       </c>
       <c r="E12">
         <v>60.999099999999999</v>
@@ -2908,7 +2908,7 @@
         <v>151.00020000000001</v>
       </c>
       <c r="D13">
-        <v>328.00060000000002</v>
+        <v>545.14980000000003</v>
       </c>
       <c r="E13">
         <v>68.006799999999998</v>
@@ -2926,7 +2926,7 @@
         <v>168.99979999999999</v>
       </c>
       <c r="D14">
-        <v>365.00139999999999</v>
+        <v>591.87840000000006</v>
       </c>
       <c r="E14">
         <v>74.998400000000004</v>
@@ -2944,7 +2944,7 @@
         <v>182.98009999999999</v>
       </c>
       <c r="D15">
-        <v>404.09059999999999</v>
+        <v>646.94870000000003</v>
       </c>
       <c r="E15">
         <v>87.000299999999996</v>
@@ -2962,7 +2962,7 @@
         <v>214.99950000000001</v>
       </c>
       <c r="D16">
-        <v>425.50650000000002</v>
+        <v>698.91499999999996</v>
       </c>
       <c r="E16">
         <v>88.003900000000002</v>
@@ -2980,7 +2980,7 @@
         <v>224.20840000000001</v>
       </c>
       <c r="D17">
-        <v>457.00220000000002</v>
+        <v>752.89819999999997</v>
       </c>
       <c r="E17">
         <v>94.997</v>
@@ -2998,7 +2998,7 @@
         <v>219.00710000000001</v>
       </c>
       <c r="D18">
-        <v>487.03809999999999</v>
+        <v>804.10159999999996</v>
       </c>
       <c r="E18">
         <v>99.967200000000005</v>
@@ -3016,7 +3016,7 @@
         <v>227.9708</v>
       </c>
       <c r="D19">
-        <v>517.99919999999997</v>
+        <v>863.16390000000001</v>
       </c>
       <c r="E19">
         <v>103.99760000000001</v>
@@ -3034,7 +3034,7 @@
         <v>241.0051</v>
       </c>
       <c r="D20">
-        <v>545.10059999999999</v>
+        <v>910.42470000000003</v>
       </c>
       <c r="E20">
         <v>111.99890000000001</v>
@@ -3052,7 +3052,7 @@
         <v>252.7825</v>
       </c>
       <c r="D21">
-        <v>584.78219999999999</v>
+        <v>966.05039999999997</v>
       </c>
       <c r="E21">
         <v>118.9987</v>
@@ -3070,7 +3070,7 @@
         <v>264.99759999999998</v>
       </c>
       <c r="D22">
-        <v>622.99599999999998</v>
+        <v>1017.2333</v>
       </c>
       <c r="E22">
         <v>153.0333</v>

</xml_diff>